<commit_message>
Components, I2C and testcode
</commit_message>
<xml_diff>
--- a/Documents/Farnel-list 2.xlsx
+++ b/Documents/Farnel-list 2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Estimated needs:</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t xml:space="preserve">Connecting leds </t>
+  </si>
+  <si>
+    <t>3 way dipswitches</t>
+  </si>
+  <si>
+    <t>adressing for leds</t>
+  </si>
+  <si>
+    <t>http://nl.farnell.com/omron-electronic-components/a6s3102h/switch-dip-3-way-sealed/dp/1960896</t>
+  </si>
+  <si>
+    <t>Ledstrip connector</t>
+  </si>
+  <si>
+    <t>to connect strip to board</t>
+  </si>
+  <si>
+    <t>http://fi.farnell.com/phoenix-contact/ptf-0-3-4-wb-1-8-h/plug-in-connector-pcb-4way-w-wires/dp/2365432?ost=ledstrip&amp;categoryId=700000005017</t>
   </si>
 </sst>
 </file>
@@ -931,7 +949,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,20 +1050,36 @@
       <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="16"/>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="16"/>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="17">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1112,10 +1146,14 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="96" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>